<commit_message>
campaign target trait level
</commit_message>
<xml_diff>
--- a/Datorama_Trait_Hierarchcial.xlsx
+++ b/Datorama_Trait_Hierarchcial.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TraitDelivery_AdvertiserID" sheetId="3" r:id="rId1"/>
     <sheet name="TraitDelivery_CampaignID" sheetId="4" r:id="rId2"/>
+    <sheet name="TraitDelivery_CampaignTargetID" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="22">
   <si>
     <t>sourceColumn</t>
   </si>
@@ -85,6 +86,12 @@
   </si>
   <si>
     <t>campaign_id</t>
+  </si>
+  <si>
+    <t>Line Item ID</t>
+  </si>
+  <si>
+    <t>Campaign_Target_ID</t>
   </si>
 </sst>
 </file>
@@ -546,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -646,5 +653,113 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
trait id for trait level
</commit_message>
<xml_diff>
--- a/Datorama_Trait_Hierarchcial.xlsx
+++ b/Datorama_Trait_Hierarchcial.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TraitDelivery_AdvertiserID" sheetId="3" r:id="rId1"/>
     <sheet name="TraitDelivery_CampaignID" sheetId="4" r:id="rId2"/>
     <sheet name="TraitDelivery_CampaignTargetID" sheetId="5" r:id="rId3"/>
+    <sheet name="TraitDelivery_TraitID" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="24">
   <si>
     <t>sourceColumn</t>
   </si>
@@ -92,6 +93,12 @@
   </si>
   <si>
     <t>Campaign_Target_ID</t>
+  </si>
+  <si>
+    <t>Segment ID</t>
+  </si>
+  <si>
+    <t>trait_id</t>
   </si>
 </sst>
 </file>
@@ -661,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -761,5 +768,113 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
trait id for conversion for trait level
</commit_message>
<xml_diff>
--- a/Datorama_Trait_Hierarchcial.xlsx
+++ b/Datorama_Trait_Hierarchcial.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TraitDelivery_AdvertiserID" sheetId="3" r:id="rId1"/>
     <sheet name="TraitDelivery_CampaignID" sheetId="4" r:id="rId2"/>
     <sheet name="TraitDelivery_CampaignTargetID" sheetId="5" r:id="rId3"/>
     <sheet name="TraitDelivery_TraitID" sheetId="6" r:id="rId4"/>
+    <sheet name="TraitCon_TraitID" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="29">
   <si>
     <t>sourceColumn</t>
   </si>
@@ -99,6 +100,21 @@
   </si>
   <si>
     <t>trait_id</t>
+  </si>
+  <si>
+    <t>total_click_based_conversion</t>
+  </si>
+  <si>
+    <t>total_view_based_conversion</t>
+  </si>
+  <si>
+    <t>Trait Click Based Conversions</t>
+  </si>
+  <si>
+    <t>Trait View Based Conversions</t>
+  </si>
+  <si>
+    <t>category_id</t>
   </si>
 </sst>
 </file>
@@ -776,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -876,5 +892,97 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>